<commit_message>
Modified trailer info to include tt in front of imdb_id in trailer_url.  Added sampleData to load by default.
</commit_message>
<xml_diff>
--- a/utils/trailers.xlsx
+++ b/utils/trailers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fec\db work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fec\betacritic\bill-morelike-component\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D55A99C-67F3-45EF-B973-27DF22ACF520}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333834F8-8281-4502-8A05-E9BAB7631388}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF11567A-78C4-44C9-96C1-C21AFE741701}"/>
   </bookViews>
@@ -1700,79 +1700,79 @@
     <t>https://s3-us-west-1.amazonaws.com/mctrailers/pulp-fiction/930074116.jpg</t>
   </si>
   <si>
-    <t>https://www.imdb.com/title/0068646/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0111161/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0081398/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0034583/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0033467/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0031381/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0032138/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0056172/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0054215/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0109830/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0059742/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0050083/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0055614/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0076759/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0062622/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0083866/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0045152/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0167260/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0066921/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0073195/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0060196/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0107290/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0075860/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0061722/videogallery</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/0110912/videogallery</t>
+    <t>https://www.imdb.com/title/tt0068646/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0111161/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0081398/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0034583/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0033467/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0031381/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0032138/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0056172/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0054215/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0109830/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0059742/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0050083/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0055614/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0076759/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0062622/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0083866/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0045152/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0167260/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0066921/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0073195/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0060196/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0107290/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0075860/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0061722/videogallery</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0110912/videogallery</t>
   </si>
 </sst>
 </file>

</xml_diff>